<commit_message>
Add TC_LF_001 to 015
</commit_message>
<xml_diff>
--- a/testcases/TutorialsNinja-Web - Test Cases.xlsx
+++ b/testcases/TutorialsNinja-Web - Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Testing\TutorialsNinjaProject\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C799FB-953D-42E6-95DE-055C9C118145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B726A773-8D0F-489C-AE5B-3527D6762384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="914" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="914" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vesion History" sheetId="2" r:id="rId1"/>
@@ -8163,7 +8163,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8192,8 +8192,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8215,6 +8221,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8388,7 +8400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -8508,6 +8520,34 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -20419,8 +20459,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20947,59 +20987,59 @@
       <c r="J19" s="33"/>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:11" s="56" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="9" t="s">
+      <c r="F20" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:11" ht="137.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="54"/>
+    </row>
+    <row r="21" spans="1:11" s="56" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="9" t="s">
+      <c r="F21" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="6"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="54"/>
     </row>
     <row r="22" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
@@ -23077,8 +23117,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23524,32 +23564,32 @@
       <c r="J16" s="33"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:11" s="49" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="47" t="s">
         <v>197</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="9" t="s">
+      <c r="F17" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="47" t="s">
         <v>199</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="6"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="48"/>
     </row>
     <row r="18" spans="1:11" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">

</xml_diff>